<commit_message>
Added new test cases for Product Code, WLTP data
</commit_message>
<xml_diff>
--- a/Test Cases Task.xlsx
+++ b/Test Cases Task.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9764a82abbeab059/Desktop/Proshore Task/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\QualityHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="8_{BDB6B31C-ABCD-40FF-B90B-567B4F9971F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03A19561-66EA-43EF-BD8C-45521905F597}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1DC5D6-A970-4593-AF8B-73506B10FBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{A09E1954-0238-4C07-B8E4-164952D08151}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{A09E1954-0238-4C07-B8E4-164952D08151}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="112">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -125,9 +126,6 @@
   </si>
   <si>
     <t>Input a Product Code Name</t>
-  </si>
-  <si>
-    <t>Select option from Code Type</t>
   </si>
   <si>
     <t>Select option from Feasibility Type</t>
@@ -140,9 +138,6 @@
 2. After product code is created Product will have unique Product code ID</t>
   </si>
   <si>
-    <t>Upon putting cursor on MasterCode field, example for inputs should be displayed (Like Eg: P01, U90)</t>
-  </si>
-  <si>
     <t>Verify Product Name is required field</t>
   </si>
   <si>
@@ -155,9 +150,6 @@
     <t>Select Feasibility Type from dropdown list with options: Model Variant, Code String</t>
   </si>
   <si>
-    <t>Select one Product Code from dropdown List of existing product codes</t>
-  </si>
-  <si>
     <t>Input BodyBuilder value</t>
   </si>
   <si>
@@ -191,12 +183,6 @@
     <t>Check WLTP Relevancy [Checkbox option Yes/No]</t>
   </si>
   <si>
-    <t>Verify Feasibity Data can be created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On user dashboard/Left Navigation Menu, Click on "Create Feasibility Data" button </t>
-  </si>
-  <si>
     <t>Verify product code is required field</t>
   </si>
   <si>
@@ -209,36 +195,12 @@
     <t>Input a valid Frontal Area</t>
   </si>
   <si>
-    <t>Navigate to the Add WLTP Data form</t>
-  </si>
-  <si>
     <t>Select an existing product code from the dropdown</t>
   </si>
   <si>
     <t>Click the "Save WLTP Data" button</t>
   </si>
   <si>
-    <t>Add WLTP Data When WLTP Relevancy is Not Checked</t>
-  </si>
-  <si>
-    <t>Select an existing product code with WLTP Relevancy set to "No"</t>
-  </si>
-  <si>
-    <t>Attempt to enter a value for Frontal Area</t>
-  </si>
-  <si>
-    <t>Create Dimensions</t>
-  </si>
-  <si>
-    <t>Add Vehicle Dimensions for Base Code Type</t>
-  </si>
-  <si>
-    <t>Verify that vehicle dimensions can be added when Code Type is Base</t>
-  </si>
-  <si>
-    <t>Navigate to the Add Dimensions form</t>
-  </si>
-  <si>
     <t>Select an existing product code with Code Type "Base"</t>
   </si>
   <si>
@@ -248,16 +210,7 @@
     <t>Click the "Save Dimensions" button</t>
   </si>
   <si>
-    <t>Add Bodybuilding Dimensions for Variant Code Type</t>
-  </si>
-  <si>
-    <t>Verify that bodybuilding dimensions can be added when Code Type is Variant</t>
-  </si>
-  <si>
     <t>Click the "Save Dimensions" button.</t>
-  </si>
-  <si>
-    <t>Select an existing product code with Code Type "Variant"</t>
   </si>
   <si>
     <t>Enter valid Bodybuilding Length, Width, and Height</t>
@@ -339,9 +292,6 @@
 2. After product code is created Product had  unique Product code ID</t>
   </si>
   <si>
-    <t>Verify  Feasibility Data can be created</t>
-  </si>
-  <si>
     <t>Select a Product Code from dropdown List of existing product codes</t>
   </si>
   <si>
@@ -369,14 +319,77 @@
     <t>1. Options for Feasibility Type are Model Variant and Code String</t>
   </si>
   <si>
-    <t>Click Save Product button without entering Product Name</t>
+    <t>Click Save Feasibility data button without entering Product Name</t>
+  </si>
+  <si>
+    <t>On user dashboard page or WLTP  Data page click on "Create WLTP Data" button</t>
+  </si>
+  <si>
+    <t>Select Yes or No WLTP Relevancy dropdown</t>
+  </si>
+  <si>
+    <t>Verify user can enter "Frontal Area" value when WLTP Relevancy is Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input "Frontal Area" </t>
+  </si>
+  <si>
+    <t>Verify "Frontal Area" is interger field</t>
+  </si>
+  <si>
+    <t>1. Input character and string
+2. Input only interger value</t>
+  </si>
+  <si>
+    <t>1. Frontal area was string instead of integer</t>
+  </si>
+  <si>
+    <t>Add Vehicle Dimensions When Code Type for selected product code is Base</t>
+  </si>
+  <si>
+    <t>Verify Vehicle Dimensions fields only appear when Code Type for selected product code is Base</t>
+  </si>
+  <si>
+    <t>Input Vehicle Dimensions based on Product Code Type: Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input Bodybuilding Dimensions based on Product Code Type: </t>
+  </si>
+  <si>
+    <t>Add Bodybuilding Dimensions if Code Type isn't Base</t>
+  </si>
+  <si>
+    <t>Select option from Code Type value: Base or None</t>
+  </si>
+  <si>
+    <t>Verify Feasibility Data can be created</t>
+  </si>
+  <si>
+    <t>Add Bodybuilding Dimensions if Code Type is None</t>
+  </si>
+  <si>
+    <t>Click Save Feasibility data button without selecting Product code from dropdown</t>
+  </si>
+  <si>
+    <t>1. Product Code should have *
+2. When user Clicks Save Feasibility data button without selecting Product code from dropdown, error message: Product Code is required should be displayed</t>
+  </si>
+  <si>
+    <t>1. Product Code had  *
+2. When user Clicked Save Feasibility data button without selecting Product code from dropdown, error message: Product Code is required was displayed</t>
+  </si>
+  <si>
+    <t>1. When user clicks on "Create WLTP Data" button Add WLTP Data form is displayed</t>
+  </si>
+  <si>
+    <t>1. When user clicks on "Create WLTP Data" button Add WLTP Data form should be displayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,8 +432,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,12 +455,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,18 +562,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -570,22 +589,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,26 +915,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A26BDFC-8492-4D89-B525-8EA4F851ADDE}">
-  <dimension ref="A2:N71"/>
+  <dimension ref="A2:R73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.06640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.06640625" style="6"/>
     <col min="9" max="9" width="28.796875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.06640625" style="6"/>
-    <col min="12" max="12" width="35.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.06640625" style="6"/>
+    <col min="12" max="12" width="35.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
@@ -938,15 +949,15 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="F4" s="6" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -954,97 +965,100 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="10">
+      <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
       <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A6" s="10">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="10">
+      <c r="A7" s="7">
         <v>3</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="10">
+      <c r="A8" s="7">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15" t="s">
+      <c r="H11" s="8"/>
+      <c r="I11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
     </row>
     <row r="12" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A12" s="6">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
+      </c>
+      <c r="L12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
@@ -1054,90 +1068,173 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D16" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="D17" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="114" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="114" x14ac:dyDescent="0.45">
       <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="71.25" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+      <c r="L18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="C22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="19">
+        <v>3</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D22" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="20"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+    </row>
+    <row r="24" spans="1:18" ht="57" x14ac:dyDescent="0.45">
       <c r="C24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L24" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="6" t="s">
+      <c r="G26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+    </row>
+    <row r="29" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="D30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>5</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>23</v>
       </c>
@@ -1145,194 +1242,295 @@
         <v>27</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>6</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D34" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D35" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D36" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="D37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+    </row>
+    <row r="40" spans="1:18" ht="57" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D44" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D34" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D35" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D36" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D37" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B39" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="1" t="s">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D46" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D47" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>8</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+    </row>
+    <row r="53" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D54" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D55" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D40" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D41" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D42" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D43" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D44" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D45" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D46" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C48" s="1" t="s">
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D56" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D57" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D58" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D62" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B50" s="6" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C66" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>12</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="1" t="s">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D68" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="1" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D69" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>13</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D73" s="1" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D51" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D52" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D53" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C56" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D57" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D58" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D59" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B61" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C62" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D63" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D64" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D65" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C67" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C68" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D69" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D70" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D71" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1349,85 +1547,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA646A2B-748D-45E9-BBD1-8DF55B1F2AE1}">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:R103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.06640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.06640625" style="6"/>
     <col min="9" max="9" width="36.73046875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.06640625" style="6"/>
-    <col min="12" max="12" width="35.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.06640625" style="6"/>
+    <col min="12" max="12" width="35.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="6">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>91</v>
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
@@ -1437,22 +1632,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="114" x14ac:dyDescent="0.45">
@@ -1460,65 +1655,71 @@
         <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>91</v>
+        <v>63</v>
+      </c>
+      <c r="L8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>2</v>
+      </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="19">
+        <v>3</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="G12" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>90</v>
+      <c r="D12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="G12" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="57" x14ac:dyDescent="0.45">
       <c r="C14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
         <v>75</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
@@ -1526,42 +1727,48 @@
         <v>19</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="19" spans="2:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="19" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+      <c r="L19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
       <c r="D20" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1569,234 +1776,248 @@
         <v>27</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+      <c r="L21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D24" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D25" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="D27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="30" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D33" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D34" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D35" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="D27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="1" t="s">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D36" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D37" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="43" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D44" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D45" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D46" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D47" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D48" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C50" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="I28" s="21"/>
-    </row>
-    <row r="30" spans="2:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G30" s="1" t="s">
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="D52" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C56" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C57" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D31" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G31" s="1" t="s">
+      <c r="D57" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="D58" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="D59" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C62" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D33" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D34" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D35" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D36" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D37" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C39" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B41" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="D62" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="D63" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D42" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D43" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D44" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C47" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D48" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D49" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D50" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B52" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C53" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D54" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D55" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D56" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C58" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C59" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D60" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D61" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D62" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
+    <row r="65" ht="22.15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1162D1DE-D107-44AA-8F72-E46C9B070DF2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>